<commit_message>
All demo tables are now exported to Sexy. Added code to allow tables not to have to script to Sexy,
</commit_message>
<xml_diff>
--- a/tables/users.demo.xlsx
+++ b/tables/users.demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\rococo\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D382E765-AF3E-4C86-BDB8-4C9B7E9BCE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFFD5BE-E29B-48AC-9CF3-3D2E21EC6A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00195B25-CB3D-43E0-A5F7-350564E66F68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>string</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>IUsers</t>
+  </si>
+  <si>
+    <t>tables\rococo.tables.test.sxh</t>
+  </si>
+  <si>
+    <t>Sexy Header</t>
   </si>
 </sst>
 </file>
@@ -700,10 +706,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,6 +813,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>